<commit_message>
Rename 'HCFC Status' to 'Status' in BP
</commit_message>
<xml_diff>
--- a/core/api/tests/files/Test_BP2025-2027.xlsx
+++ b/core/api/tests/files/Test_BP2025-2027.xlsx
@@ -39,7 +39,7 @@
     <t xml:space="preserve">Agency</t>
   </si>
   <si>
-    <t xml:space="preserve">HCFC Status</t>
+    <t xml:space="preserve">Status</t>
   </si>
   <si>
     <t xml:space="preserve">Type</t>
@@ -2434,8 +2434,8 @@
   </sheetPr>
   <dimension ref="A1:AH652"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="AA1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AC4" activeCellId="0" sqref="AC4"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.859375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
Rename 'HCFC Status' to 'Status' in BP (#677)
</commit_message>
<xml_diff>
--- a/core/api/tests/files/Test_BP2025-2027.xlsx
+++ b/core/api/tests/files/Test_BP2025-2027.xlsx
@@ -39,7 +39,7 @@
     <t xml:space="preserve">Agency</t>
   </si>
   <si>
-    <t xml:space="preserve">HCFC Status</t>
+    <t xml:space="preserve">Status</t>
   </si>
   <si>
     <t xml:space="preserve">Type</t>
@@ -2434,8 +2434,8 @@
   </sheetPr>
   <dimension ref="A1:AH652"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="AA1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AC4" activeCellId="0" sqref="AC4"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.859375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
BP export: updates to columns names
</commit_message>
<xml_diff>
--- a/core/api/tests/files/Test_BP2025-2027.xlsx
+++ b/core/api/tests/files/Test_BP2025-2027.xlsx
@@ -69,52 +69,52 @@
     <t xml:space="preserve">Required by Model</t>
   </si>
   <si>
-    <t xml:space="preserve">Value ($000) 2025 adjusted</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ODP 2025 adjusted</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MT for HFC 2025 adjusted</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CO2-EQ 2025 adjusted</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Value ($000) 2026 adjusted</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ODP 2026 adjusted</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MT for HFC 2026 adjusted</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CO2-EQ 2026 adjusted</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Value ($000) 2027 adjusted</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ODP 2027 adjusted</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MT for HFC 2027 adjusted</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CO2-EQ 2027 adjusted</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Value ($000) after 2027 adjusted</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ODP after 2027 adjusted</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MT for HFC after 2027 adjusted</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CO2-EQ after 2027 adjusted</t>
+    <t xml:space="preserve">Value (US $) 2025</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ODP 2025</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MT for HFC 2025</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CO2-EQ 2025 tonnes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Value (US $) 2026</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ODP 2026</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MT for HFC 2026</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CO2-EQ 2026 tonnes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Value (US $) 2027</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ODP 2027</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MT for HFC 2027</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CO2-EQ 2027 tonnes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Value (US $) after 2027</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ODP after 2027</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MT for HFC after 2027</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CO2-EQ after 2027 tonnes</t>
   </si>
   <si>
     <t xml:space="preserve">Project Status (A/P)</t>
@@ -2434,8 +2434,8 @@
   </sheetPr>
   <dimension ref="A1:AH652"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="M1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="R1" activeCellId="0" sqref="R1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.859375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
Add filter for 'All agencies' (#736)
* Add filter for 'All agencies'

* BP export: updates to columns names

* Use iso3 country value in bp activity id
</commit_message>
<xml_diff>
--- a/core/api/tests/files/Test_BP2025-2027.xlsx
+++ b/core/api/tests/files/Test_BP2025-2027.xlsx
@@ -69,52 +69,52 @@
     <t xml:space="preserve">Required by Model</t>
   </si>
   <si>
-    <t xml:space="preserve">Value ($000) 2025 adjusted</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ODP 2025 adjusted</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MT for HFC 2025 adjusted</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CO2-EQ 2025 adjusted</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Value ($000) 2026 adjusted</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ODP 2026 adjusted</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MT for HFC 2026 adjusted</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CO2-EQ 2026 adjusted</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Value ($000) 2027 adjusted</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ODP 2027 adjusted</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MT for HFC 2027 adjusted</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CO2-EQ 2027 adjusted</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Value ($000) after 2027 adjusted</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ODP after 2027 adjusted</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MT for HFC after 2027 adjusted</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CO2-EQ after 2027 adjusted</t>
+    <t xml:space="preserve">Value (US $) 2025</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ODP 2025</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MT for HFC 2025</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CO2-EQ 2025 tonnes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Value (US $) 2026</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ODP 2026</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MT for HFC 2026</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CO2-EQ 2026 tonnes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Value (US $) 2027</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ODP 2027</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MT for HFC 2027</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CO2-EQ 2027 tonnes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Value (US $) after 2027</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ODP after 2027</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MT for HFC after 2027</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CO2-EQ after 2027 tonnes</t>
   </si>
   <si>
     <t xml:space="preserve">Project Status (A/P)</t>
@@ -2434,8 +2434,8 @@
   </sheetPr>
   <dimension ref="A1:AH652"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="M1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="R1" activeCellId="0" sqref="R1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.859375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>